<commit_message>
changes files to webp
</commit_message>
<xml_diff>
--- a/resources/data/events/Jahresplanung SPD Albstadt für die Homepage.xlsx
+++ b/resources/data/events/Jahresplanung SPD Albstadt für die Homepage.xlsx
@@ -434,7 +434,7 @@
         <v>Wer sorgt für unsere Sicherheit? Was muss sich ändern? Die Bundeswehr ist ein Teil der Antwort. Ein Teil, der in diesen Zeiten wichtiger geworden ist, da wir Krieg in Europa erleben. Nur in welchem Zustand ist die Bundeswehr eigentlich? Darüber möchten wir sprechen mit Dr. Eva Högl, Wehrbeauftragte des Deutschen Bundestages, Wolfgang Schneiderhan General a.D  von 2002 bis 2009 Generalinspekteur der Bundeswehr und Robin Mesarosch MdB</v>
       </c>
       <c r="E2" t="str">
-        <v>/resources/images/stadthalle.JPG</v>
+        <v>/resources/images/stadthalle.webp</v>
       </c>
     </row>
     <row r="3" xml:space="preserve">
@@ -546,7 +546,7 @@
         <v>Am 9. Juni 2024 ist Kommunal- und Europawahl. Unterstützen Sie die Zukunft von Albstadt und Europa! Ihre Stimme zählt – wählen Sie die Kandidaten der SPD Albstadt für die Kommunalwahl und setzen Sie Ihr Kreuz auch bei der SPD für die Europawahl.</v>
       </c>
       <c r="E8" t="str">
-        <v>/resources/images/news/rathaus.jpg</v>
+        <v>/resources/images/news/rathaus.webp</v>
       </c>
     </row>
     <row r="9">
@@ -560,7 +560,7 @@
         <v xml:space="preserve">An diesem Abendtreffen kommen alle zusammen, um auf die vergangenen Wochen zurückzublicken, die ganz im Zeichen der Kommunalwahl standen. </v>
       </c>
       <c r="E9" t="str">
-        <v>/resources/images/news/rathaus.jpg</v>
+        <v>/resources/images/news/rathaus.webp</v>
       </c>
     </row>
     <row r="10" xml:space="preserve">

</xml_diff>